<commit_message>
[MEBA] Spanish original in english
</commit_message>
<xml_diff>
--- a/changes-guide.xlsx
+++ b/changes-guide.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB632DA-6338-4540-9272-03C3005A7122}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31F9C51-85D1-4DF5-ACC7-25D4634F5606}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{5068E5B8-477E-40A4-BCFA-31527DB741B5}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="324">
   <si>
     <t>Saruman</t>
   </si>
@@ -781,9 +781,6 @@
     <t>The Under-leas (Hero version</t>
   </si>
   <si>
-    <t>Playable any moment</t>
-  </si>
-  <si>
     <t>Woses of Eryn Vorn (minion version</t>
   </si>
   <si>
@@ -992,6 +989,12 @@
   </si>
   <si>
     <t>Pilfer Anything Unwatched</t>
+  </si>
+  <si>
+    <t>CRF Challenge Errata - healing effects</t>
+  </si>
+  <si>
+    <t>Playable any moment. Hazard limit</t>
   </si>
 </sst>
 </file>
@@ -1347,8 +1350,8 @@
   <dimension ref="A1:I289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H263" sqref="H263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,10 +1377,10 @@
         <v>55</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>210</v>
@@ -1454,7 +1457,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1463,7 +1466,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I6" s="3"/>
     </row>
@@ -1563,7 +1566,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I12" s="3"/>
     </row>
@@ -1646,7 +1649,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1656,7 +1659,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1725,7 +1728,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1734,7 +1737,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I23" s="3"/>
     </row>
@@ -1755,7 +1758,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1764,7 +1767,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I25" s="3"/>
     </row>
@@ -1832,7 +1835,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1841,13 +1844,13 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1856,7 +1859,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I31" s="3"/>
     </row>
@@ -1879,7 +1882,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1889,12 +1892,12 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1903,7 +1906,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I34" s="3"/>
     </row>
@@ -1958,7 +1961,7 @@
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -2048,7 +2051,7 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I43" s="3"/>
     </row>
@@ -2080,7 +2083,7 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I45" s="3"/>
     </row>
@@ -2150,7 +2153,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -2177,7 +2180,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2197,11 +2200,11 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -2227,7 +2230,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -2236,7 +2239,7 @@
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I55" s="3"/>
     </row>
@@ -2334,7 +2337,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -2344,7 +2347,7 @@
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2381,7 +2384,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="1" t="s">
@@ -2413,7 +2416,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -2455,7 +2458,7 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -2520,7 +2523,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -2529,7 +2532,7 @@
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="H74" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I74" s="3"/>
     </row>
@@ -2819,7 +2822,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -2828,7 +2831,7 @@
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
       <c r="H93" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I93" s="3"/>
     </row>
@@ -3022,13 +3025,13 @@
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
       <c r="H105" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I105" s="3"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -3037,7 +3040,7 @@
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
       <c r="H106" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I106" s="3"/>
     </row>
@@ -3259,7 +3262,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -3274,12 +3277,12 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E122" s="3"/>
       <c r="F122" s="3"/>
@@ -3289,7 +3292,7 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -3298,7 +3301,7 @@
       <c r="F123" s="3"/>
       <c r="G123" s="3"/>
       <c r="H123" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I123" s="3"/>
     </row>
@@ -3351,7 +3354,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -3360,7 +3363,7 @@
       <c r="F127" s="3"/>
       <c r="G127" s="3"/>
       <c r="H127" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I127" s="3"/>
     </row>
@@ -3415,11 +3418,11 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B131" s="3"/>
       <c r="C131" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D131" s="3"/>
       <c r="E131" s="3"/>
@@ -3460,7 +3463,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
@@ -3470,7 +3473,7 @@
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
       <c r="I134" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -3507,7 +3510,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
@@ -3522,7 +3525,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>54</v>
@@ -3586,11 +3589,11 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B142" s="3"/>
       <c r="C142" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D142" s="3"/>
       <c r="E142" s="3"/>
@@ -3631,7 +3634,7 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
@@ -3641,7 +3644,7 @@
       <c r="G145" s="3"/>
       <c r="H145" s="3"/>
       <c r="I145" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -3661,7 +3664,7 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
@@ -3736,7 +3739,7 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
@@ -3745,7 +3748,7 @@
       <c r="F152" s="3"/>
       <c r="G152" s="3"/>
       <c r="H152" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I152" s="3"/>
     </row>
@@ -3828,7 +3831,7 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
@@ -3858,11 +3861,11 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B160" s="3"/>
       <c r="C160" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D160" s="3"/>
       <c r="E160" s="3"/>
@@ -3873,7 +3876,7 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
@@ -3882,7 +3885,7 @@
       <c r="F161" s="3"/>
       <c r="G161" s="3"/>
       <c r="H161" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I161" s="3"/>
     </row>
@@ -3932,12 +3935,12 @@
       <c r="G164" s="3"/>
       <c r="H164" s="3"/>
       <c r="I164" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
@@ -3946,7 +3949,7 @@
       <c r="F165" s="3"/>
       <c r="G165" s="3"/>
       <c r="H165" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I165" s="3"/>
     </row>
@@ -3984,7 +3987,7 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
@@ -3993,7 +3996,7 @@
       <c r="F168" s="3"/>
       <c r="G168" s="3"/>
       <c r="H168" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I168" s="3"/>
     </row>
@@ -4031,7 +4034,7 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
@@ -4040,17 +4043,17 @@
       <c r="F171" s="3"/>
       <c r="G171" s="3"/>
       <c r="H171" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I171" s="3"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B172" s="3"/>
       <c r="C172" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D172" s="3"/>
       <c r="E172" s="3"/>
@@ -4098,7 +4101,7 @@
       </c>
       <c r="C175" s="3"/>
       <c r="D175" s="1" t="s">
-        <v>242</v>
+        <v>322</v>
       </c>
       <c r="E175" s="3"/>
       <c r="F175" s="3"/>
@@ -4172,13 +4175,13 @@
       </c>
       <c r="G179" s="3"/>
       <c r="H179" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I179" s="3"/>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
@@ -4187,7 +4190,7 @@
       <c r="F180" s="3"/>
       <c r="G180" s="3"/>
       <c r="H180" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I180" s="3"/>
     </row>
@@ -4238,11 +4241,11 @@
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B184" s="3"/>
       <c r="C184" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D184" s="3"/>
       <c r="E184" s="3"/>
@@ -4253,7 +4256,7 @@
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
@@ -4262,7 +4265,7 @@
       <c r="F185" s="3"/>
       <c r="G185" s="3"/>
       <c r="H185" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I185" s="3"/>
     </row>
@@ -4426,7 +4429,7 @@
       </c>
       <c r="B196" s="3"/>
       <c r="C196" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D196" s="1" t="s">
         <v>54</v>
@@ -4452,7 +4455,7 @@
       <c r="F197" s="3"/>
       <c r="G197" s="3"/>
       <c r="H197" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I197" s="3"/>
     </row>
@@ -4633,7 +4636,7 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B209" s="3"/>
       <c r="C209" s="3"/>
@@ -4642,13 +4645,13 @@
       <c r="F209" s="3"/>
       <c r="G209" s="3"/>
       <c r="H209" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I209" s="3"/>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B210" s="3"/>
       <c r="C210" s="3"/>
@@ -4687,7 +4690,7 @@
       <c r="F212" s="3"/>
       <c r="G212" s="3"/>
       <c r="H212" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I212" s="3"/>
     </row>
@@ -4705,7 +4708,7 @@
       <c r="G213" s="3"/>
       <c r="H213" s="3"/>
       <c r="I213" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
@@ -4725,7 +4728,7 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B215" s="3"/>
       <c r="C215" s="3"/>
@@ -4734,7 +4737,7 @@
       <c r="F215" s="3"/>
       <c r="G215" s="3"/>
       <c r="H215" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I215" s="3"/>
     </row>
@@ -4964,7 +4967,7 @@
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B230" s="3"/>
       <c r="C230" s="3"/>
@@ -4974,7 +4977,7 @@
       <c r="G230" s="3"/>
       <c r="H230" s="3"/>
       <c r="I230" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
@@ -5013,7 +5016,7 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B233" s="3"/>
       <c r="C233" s="3"/>
@@ -5024,13 +5027,13 @@
       <c r="F233" s="3"/>
       <c r="G233" s="3"/>
       <c r="H233" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I233" s="3"/>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B234" s="3"/>
       <c r="C234" s="3"/>
@@ -5039,7 +5042,7 @@
       <c r="F234" s="3"/>
       <c r="G234" s="3"/>
       <c r="H234" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I234" s="3"/>
     </row>
@@ -5075,7 +5078,7 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B237" s="3"/>
       <c r="C237" s="3"/>
@@ -5084,7 +5087,7 @@
       <c r="F237" s="3"/>
       <c r="G237" s="3"/>
       <c r="H237" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I237" s="3"/>
     </row>
@@ -5103,7 +5106,7 @@
       <c r="F238" s="3"/>
       <c r="G238" s="3"/>
       <c r="H238" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I238" s="3"/>
     </row>
@@ -5141,7 +5144,7 @@
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B241" s="3"/>
       <c r="C241" s="3"/>
@@ -5171,7 +5174,7 @@
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B243" s="3"/>
       <c r="C243" s="3"/>
@@ -5180,7 +5183,7 @@
       <c r="F243" s="3"/>
       <c r="G243" s="3"/>
       <c r="H243" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I243" s="3"/>
     </row>
@@ -5216,11 +5219,11 @@
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B246" s="3"/>
       <c r="C246" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D246" s="3"/>
       <c r="E246" s="3"/>
@@ -5280,7 +5283,7 @@
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B250" s="3"/>
       <c r="C250" s="3"/>
@@ -5289,7 +5292,7 @@
       <c r="F250" s="3"/>
       <c r="G250" s="3"/>
       <c r="H250" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I250" s="3"/>
     </row>
@@ -5321,10 +5324,10 @@
       <c r="F252" s="3"/>
       <c r="G252" s="3"/>
       <c r="H252" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I252" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.25">
@@ -5465,12 +5468,12 @@
       <c r="G261" s="3"/>
       <c r="H261" s="3"/>
       <c r="I261" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B262" s="1" t="s">
         <v>54</v>
@@ -5483,13 +5486,13 @@
       <c r="F262" s="3"/>
       <c r="G262" s="3"/>
       <c r="H262" s="1" t="s">
-        <v>252</v>
+        <v>323</v>
       </c>
       <c r="I262" s="3"/>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B263" s="3"/>
       <c r="C263" s="3"/>
@@ -5498,7 +5501,7 @@
       <c r="F263" s="3"/>
       <c r="G263" s="3"/>
       <c r="H263" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I263" s="3"/>
     </row>
@@ -5508,7 +5511,7 @@
       </c>
       <c r="B264" s="3"/>
       <c r="C264" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D264" s="3"/>
       <c r="E264" s="1" t="s">
@@ -5536,7 +5539,7 @@
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B266" s="3"/>
       <c r="C266" s="3"/>
@@ -5545,7 +5548,7 @@
       <c r="F266" s="3"/>
       <c r="G266" s="3"/>
       <c r="H266" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I266" s="3"/>
     </row>
@@ -5664,7 +5667,7 @@
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B274" s="3"/>
       <c r="C274" s="3"/>
@@ -5673,7 +5676,7 @@
       <c r="F274" s="3"/>
       <c r="G274" s="3"/>
       <c r="H274" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I274" s="3"/>
     </row>
@@ -5709,7 +5712,7 @@
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B277" s="3"/>
       <c r="C277" s="3"/>
@@ -5718,7 +5721,7 @@
       <c r="F277" s="3"/>
       <c r="G277" s="3"/>
       <c r="H277" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I277" s="3"/>
     </row>
@@ -5879,12 +5882,12 @@
         <v>243</v>
       </c>
       <c r="I287" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B288" s="1" t="s">
         <v>54</v>
@@ -5901,7 +5904,7 @@
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B289" s="3"/>
       <c r="C289" s="3"/>
@@ -5910,7 +5913,7 @@
       <c r="F289" s="3"/>
       <c r="G289" s="3"/>
       <c r="H289" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I289" s="3"/>
     </row>

</xml_diff>